<commit_message>
Implement specifying cohort (age of an item) when mutating a balance sheet item)
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE95B8F-6472-4E17-9AC7-1DA34FA5CBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AF1C47-A666-48C7-9C2B-0B8FB319E66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="5" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="65">
   <si>
     <t>Relative</t>
   </si>
@@ -225,6 +225,18 @@
   </si>
   <si>
     <t>Reference Sub Item Type</t>
+  </si>
+  <si>
+    <t>Age months</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>MinAgeMonths</t>
   </si>
 </sst>
 </file>
@@ -613,20 +625,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -634,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -642,166 +656,179 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="b">
+      <c r="E3" t="b">
         <v>0</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="b">
+      <c r="E5" t="b">
         <v>0</v>
       </c>
-      <c r="D5" t="b">
+      <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" t="b">
+      <c r="G5" t="b">
         <v>1</v>
       </c>
-      <c r="F5" t="b">
+      <c r="H5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F8" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45777</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1">
-        <v>45808</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.02</v>
+      <c r="D9" s="1">
+        <v>45777</v>
       </c>
       <c r="E9" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="2">
         <v>0.2</v>
       </c>
-      <c r="F9" s="2">
+      <c r="H9" s="2">
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1">
-        <v>45838</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="C10">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45945</v>
+      </c>
+      <c r="E11" s="2">
         <v>0.01</v>
       </c>
-      <c r="D10" s="2">
+      <c r="F11" s="2">
         <v>0.03</v>
       </c>
-      <c r="E10" s="2">
+      <c r="G11" s="2">
         <v>0.2</v>
       </c>
-      <c r="F10" s="2">
+      <c r="H11" s="2">
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="D16" s="2"/>
     </row>
@@ -824,6 +851,10 @@
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1378,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A3C72-8141-4CE1-9B29-33F3A1419413}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,7 +1445,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>46295</v>
+        <v>45930</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1449,6 +1480,20 @@
       </c>
       <c r="C5" s="4">
         <v>-200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>46356</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>20000</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve ordering of rows and columns in demo
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AF1C47-A666-48C7-9C2B-0B8FB319E66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30431690-CB6F-499A-9CD8-EF1949F76E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="5" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
-    <sheet name="interest rates" sheetId="2" r:id="rId2"/>
-    <sheet name="tax" sheetId="3" r:id="rId3"/>
-    <sheet name="audit" sheetId="4" r:id="rId4"/>
-    <sheet name="dividend" sheetId="5" r:id="rId5"/>
-    <sheet name="production" sheetId="6" r:id="rId6"/>
-    <sheet name="costs" sheetId="7" r:id="rId7"/>
+    <sheet name="production" sheetId="6" r:id="rId2"/>
+    <sheet name="interest rates" sheetId="2" r:id="rId3"/>
+    <sheet name="costs" sheetId="7" r:id="rId4"/>
+    <sheet name="tax" sheetId="3" r:id="rId5"/>
+    <sheet name="audit" sheetId="4" r:id="rId6"/>
+    <sheet name="dividend" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
   <si>
     <t>Relative</t>
   </si>
@@ -225,9 +225,6 @@
   </si>
   <si>
     <t>Reference Sub Item Type</t>
-  </si>
-  <si>
-    <t>Age months</t>
   </si>
   <si>
     <t>Book</t>
@@ -625,17 +622,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -716,48 +711,66 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45777</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.03</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
       <c r="D9" s="1">
-        <v>45777</v>
+        <v>45808</v>
       </c>
       <c r="E9" s="2">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="F9" s="2">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G9" s="2">
         <v>0.2</v>
@@ -770,17 +783,17 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="C10">
-        <v>36</v>
+      <c r="B10" t="s">
+        <v>62</v>
       </c>
       <c r="D10" s="1">
-        <v>45808</v>
+        <v>45945</v>
       </c>
       <c r="E10" s="2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F10" s="2">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="G10" s="2">
         <v>0.2</v>
@@ -790,27 +803,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="1">
-        <v>45945</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.03</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
@@ -851,10 +845,6 @@
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -862,11 +852,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A3C72-8141-4CE1-9B29-33F3A1419413}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>46037</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>-100000</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>46902</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="4">
+        <v>-200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>46356</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>20000</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408AD00A-839B-4347-BBD4-5564B7B0FB9B}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1225,12 +1307,100 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="4" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>46752</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4">
+        <v>-100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>46767</v>
+      </c>
+      <c r="E4" s="1">
+        <v>47026</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45991</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45703</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45793</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677DDE5-DC58-4FA0-9231-0F203A0C4FFF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1263,11 +1433,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D314085B-29B2-4F1C-B0E6-FF11268580B0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1313,11 +1483,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1405,188 +1575,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A3C72-8141-4CE1-9B29-33F3A1419413}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>45930</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>10000</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>46037</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4">
-        <v>-100000</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>46902</v>
-      </c>
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="4">
-        <v>-200000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>46356</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
-        <v>20000</v>
-      </c>
-      <c r="D6">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="4" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>46387</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>46752</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4">
-        <v>-100</v>
-      </c>
-      <c r="D4" s="1">
-        <v>46767</v>
-      </c>
-      <c r="E4" s="1">
-        <v>47026</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>45991</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5">
-        <v>10000</v>
-      </c>
-      <c r="D5" s="1">
-        <v>45703</v>
-      </c>
-      <c r="E5" s="1">
-        <v>45793</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Rename BalanceSheetSide column to balance_sheet_category, and have it as a classification so we can add extra logic to it
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30431690-CB6F-499A-9CD8-EF1949F76E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013F2B7C-1C58-4FF3-992D-AC0126754A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Agio</t>
   </si>
   <si>
-    <t>BalanceSheetSide</t>
-  </si>
-  <si>
     <t>Assets</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>MinAgeMonths</t>
+  </si>
+  <si>
+    <t>BalanceSheetCategory</t>
   </si>
 </sst>
 </file>
@@ -624,11 +624,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -645,7 +647,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -712,13 +714,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -738,7 +740,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1">
         <v>45777</v>
@@ -758,7 +760,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>36</v>
@@ -781,10 +783,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1">
         <v>45945</v>
@@ -868,21 +870,21 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -918,7 +920,7 @@
         <v>46902</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4">
         <v>-200000</v>
@@ -947,9 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408AD00A-839B-4347-BBD4-5564B7B0FB9B}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -961,27 +961,27 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -989,13 +989,13 @@
         <v>44926</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3">
         <v>3.0499999999999999E-2</v>
@@ -1006,13 +1006,13 @@
         <v>44926</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
       </c>
       <c r="F4" s="3">
         <v>2.9499999999999998E-2</v>
@@ -1023,13 +1023,13 @@
         <v>44926</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
       </c>
       <c r="F5" s="3">
         <v>3.1800000000000002E-2</v>
@@ -1040,13 +1040,13 @@
         <v>44926</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3">
         <v>2.86E-2</v>
@@ -1057,13 +1057,13 @@
         <v>44926</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3">
         <v>2.5499999999999998E-2</v>
@@ -1074,13 +1074,13 @@
         <v>44926</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="3">
         <v>2.6499999999999999E-2</v>
@@ -1091,13 +1091,13 @@
         <v>44926</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="3">
         <v>2.7E-2</v>
@@ -1108,16 +1108,16 @@
         <v>44926</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
       </c>
       <c r="F10" s="3">
         <v>2.8500000000000001E-2</v>
@@ -1128,16 +1128,16 @@
         <v>44926</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3">
         <v>2.5499999999999998E-2</v>
@@ -1148,13 +1148,13 @@
         <v>46387</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="3">
         <v>5.0500000000000003E-2</v>
@@ -1165,13 +1165,13 @@
         <v>46387</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
         <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
       </c>
       <c r="F13" s="3">
         <v>4.9500000000000002E-2</v>
@@ -1182,13 +1182,13 @@
         <v>46387</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
         <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
       </c>
       <c r="F14" s="3">
         <v>5.1799999999999999E-2</v>
@@ -1199,13 +1199,13 @@
         <v>46387</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="3">
         <v>4.8600000000000004E-2</v>
@@ -1216,13 +1216,13 @@
         <v>46387</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="3">
         <v>4.5499999999999999E-2</v>
@@ -1233,13 +1233,13 @@
         <v>46387</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" s="3">
         <v>4.65E-2</v>
@@ -1250,13 +1250,13 @@
         <v>46387</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="3">
         <v>4.7E-2</v>
@@ -1267,16 +1267,16 @@
         <v>46387</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
         <v>32</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>33</v>
-      </c>
-      <c r="E19" t="s">
-        <v>34</v>
       </c>
       <c r="F19" s="3">
         <v>4.8500000000000001E-2</v>
@@ -1287,16 +1287,16 @@
         <v>46387</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
         <v>32</v>
       </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" s="3">
         <v>4.5499999999999999E-2</v>
@@ -1325,24 +1325,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
         <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1350,7 +1350,7 @@
         <v>46387</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3">
         <v>-10</v>
@@ -1361,7 +1361,7 @@
         <v>46752</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4">
         <v>-100</v>
@@ -1378,7 +1378,7 @@
         <v>45991</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>10000</v>
@@ -1414,12 +1414,12 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3">
         <v>0.25700000000000001</v>
@@ -1451,12 +1451,12 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1472,10 +1472,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1487,7 +1487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1510,35 +1510,35 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1546,10 +1546,10 @@
         <v>45930</v>
       </c>
       <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1563,7 +1563,7 @@
         <v>45991</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Have liabilities and equity with positive values on the balance sheet, and output both a signed and unsigned book value.
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013F2B7C-1C58-4FF3-992D-AC0126754A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217F8BCA-18C6-4B4F-B8F9-8EDBF32636DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -625,7 +625,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,7 +857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A3C72-8141-4CE1-9B29-33F3A1419413}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -909,7 +911,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="4">
-        <v>-100000</v>
+        <v>100000</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -923,7 +925,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="4">
-        <v>-200000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1487,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Rename old and new book to backbook and frontbook
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217F8BCA-18C6-4B4F-B8F9-8EDBF32636DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75585F8B-3D5B-474B-8265-D7DFB7837903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="30984" windowHeight="16824" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -227,13 +227,13 @@
     <t>Book</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>MinAgeMonths</t>
   </si>
   <si>
     <t>BalanceSheetCategory</t>
+  </si>
+  <si>
+    <t>front</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,13 +714,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -786,7 +786,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1">
         <v>45945</v>
@@ -857,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A3C72-8141-4CE1-9B29-33F3A1419413}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -951,7 +951,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408AD00A-839B-4347-BBD4-5564B7B0FB9B}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1313,7 +1315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1401,9 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677DDE5-DC58-4FA0-9231-0F203A0C4FFF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1440,7 +1442,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1489,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1557,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="4">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1571,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="4">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor cost income rule
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75585F8B-3D5B-474B-8265-D7DFB7837903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D400D4-786D-4C85-8911-3983C39E2033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="30984" windowHeight="16824" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>Relative</t>
   </si>
@@ -203,18 +203,12 @@
     <t>Project X</t>
   </si>
   <si>
-    <t>Project Y</t>
-  </si>
-  <si>
     <t>PnL Start</t>
   </si>
   <si>
     <t>PnL End</t>
   </si>
   <si>
-    <t>Project Z</t>
-  </si>
-  <si>
     <t>Sub_Item_type</t>
   </si>
   <si>
@@ -234,6 +228,18 @@
   </si>
   <si>
     <t>front</t>
+  </si>
+  <si>
+    <t>Project A</t>
+  </si>
+  <si>
+    <t>Project B</t>
+  </si>
+  <si>
+    <t>Project C</t>
+  </si>
+  <si>
+    <t>Project D</t>
   </si>
 </sst>
 </file>
@@ -628,16 +634,16 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -645,15 +651,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>11</v>
       </c>
@@ -670,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -687,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>8</v>
       </c>
@@ -704,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>9</v>
       </c>
@@ -712,15 +718,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -738,7 +744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -758,7 +764,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -781,12 +787,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1">
         <v>45945</v>
@@ -804,47 +810,47 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="D21" s="2"/>
     </row>
@@ -858,16 +864,16 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -875,12 +881,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -889,7 +895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45930</v>
       </c>
@@ -903,7 +909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>46037</v>
       </c>
@@ -917,7 +923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>46902</v>
       </c>
@@ -928,7 +934,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>46356</v>
       </c>
@@ -955,12 +961,12 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -968,7 +974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -988,7 +994,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44926</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>3.0499999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44926</v>
       </c>
@@ -1022,7 +1028,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44926</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>3.1800000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44926</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44926</v>
       </c>
@@ -1073,7 +1079,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44926</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44926</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44926</v>
       </c>
@@ -1127,7 +1133,7 @@
         <v>2.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44926</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>46387</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>46387</v>
       </c>
@@ -1181,7 +1187,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>46387</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>46387</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>4.8600000000000004E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>46387</v>
       </c>
@@ -1232,7 +1238,7 @@
         <v>4.5499999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>46387</v>
       </c>
@@ -1249,7 +1255,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>46387</v>
       </c>
@@ -1266,7 +1272,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>46387</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>46387</v>
       </c>
@@ -1313,20 +1319,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="4" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1334,7 +1341,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1345,13 +1352,13 @@
         <v>50</v>
       </c>
       <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>46387</v>
       </c>
@@ -1362,38 +1369,72 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>46752</v>
+        <v>45658</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C4">
         <v>-100</v>
       </c>
       <c r="D4" s="1">
-        <v>46767</v>
+        <v>45672</v>
       </c>
       <c r="E4" s="1">
-        <v>47026</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45930</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45991</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>10000</v>
       </c>
       <c r="D5" s="1">
-        <v>45703</v>
+        <v>46068</v>
       </c>
       <c r="E5" s="1">
-        <v>45793</v>
+        <v>46158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>46172</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6">
+        <v>-500</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45658</v>
+      </c>
+      <c r="E6" s="1">
+        <v>46022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>46112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45658</v>
+      </c>
+      <c r="E7" s="1">
+        <v>46022</v>
       </c>
     </row>
   </sheetData>
@@ -1407,13 +1448,13 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1421,7 +1462,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1429,7 +1470,7 @@
         <v>0.25700000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -1445,12 +1486,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1458,7 +1499,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1466,7 +1507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1474,9 +1515,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -1491,20 +1532,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1512,7 +1553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1520,7 +1561,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1528,7 +1569,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1545,7 +1586,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45930</v>
       </c>
@@ -1562,7 +1603,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45991</v>
       </c>

</xml_diff>

<commit_message>
Implement mid-period revenue and expense recognition in cost income rule
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D400D4-786D-4C85-8911-3983C39E2033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441220C3-B9B5-4330-9309-5CE963EE0A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="68">
   <si>
     <t>Relative</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>Project D</t>
+  </si>
+  <si>
+    <t>Project E</t>
+  </si>
+  <si>
+    <t>Project F</t>
   </si>
 </sst>
 </file>
@@ -1319,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1435,6 +1441,40 @@
       </c>
       <c r="E7" s="1">
         <v>46022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>46174</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45717</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45961</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>46174</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>-4000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45717</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor balance sheet metrics from 'quantity' to 'nominal'
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441220C3-B9B5-4330-9309-5CE963EE0A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC960E8-EFAF-4578-A84E-9C7F1933027B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="30984" windowHeight="16824" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -179,9 +179,6 @@
     <t>retained earnings</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>offsetliquidity* Metric</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>Project F</t>
+  </si>
+  <si>
+    <t>Nominal</t>
   </si>
 </sst>
 </file>
@@ -636,9 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -647,6 +645,7 @@
     <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -659,7 +658,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -726,13 +725,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
         <v>58</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -798,7 +797,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1">
         <v>45945</v>
@@ -809,8 +808,8 @@
       <c r="F10" s="2">
         <v>0.03</v>
       </c>
-      <c r="G10" s="2">
-        <v>0.2</v>
+      <c r="G10" s="4">
+        <v>2</v>
       </c>
       <c r="H10" s="2">
         <v>0.03</v>
@@ -870,7 +869,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -884,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -892,10 +891,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -934,7 +933,7 @@
         <v>46902</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="4">
         <v>200000</v>
@@ -964,7 +963,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1327,8 +1326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1344,7 +1343,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1352,16 +1351,16 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
         <v>53</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1369,7 +1368,7 @@
         <v>46387</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3">
         <v>-10</v>
@@ -1380,7 +1379,7 @@
         <v>45658</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>-100</v>
@@ -1397,7 +1396,7 @@
         <v>45991</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>10000</v>
@@ -1414,7 +1413,7 @@
         <v>46172</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>-500</v>
@@ -1431,7 +1430,7 @@
         <v>46112</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>600</v>
@@ -1448,7 +1447,7 @@
         <v>46174</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>5000</v>
@@ -1465,7 +1464,7 @@
         <v>46174</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9">
         <v>-4000</v>
@@ -1486,7 +1485,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677DDE5-DC58-4FA0-9231-0F203A0C4FFF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1523,7 +1524,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1557,7 +1558,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -1572,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1620,10 +1621,10 @@
         <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Possibility to input manual repayment rates
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC960E8-EFAF-4578-A84E-9C7F1933027B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A860A4C0-00F4-4A36-AC2E-89445045902E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="30984" windowHeight="16824" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
-    <sheet name="production" sheetId="6" r:id="rId2"/>
-    <sheet name="interest rates" sheetId="2" r:id="rId3"/>
-    <sheet name="costs" sheetId="7" r:id="rId4"/>
-    <sheet name="tax" sheetId="3" r:id="rId5"/>
-    <sheet name="audit" sheetId="4" r:id="rId6"/>
-    <sheet name="dividend" sheetId="5" r:id="rId7"/>
+    <sheet name="intangible redemption" sheetId="8" r:id="rId2"/>
+    <sheet name="production" sheetId="6" r:id="rId3"/>
+    <sheet name="interest rates" sheetId="2" r:id="rId4"/>
+    <sheet name="costs" sheetId="7" r:id="rId5"/>
+    <sheet name="tax" sheetId="3" r:id="rId6"/>
+    <sheet name="audit" sheetId="4" r:id="rId7"/>
+    <sheet name="dividend" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
   <si>
     <t>Relative</t>
   </si>
@@ -246,6 +247,18 @@
   </si>
   <si>
     <t>Nominal</t>
+  </si>
+  <si>
+    <t>ItemType</t>
+  </si>
+  <si>
+    <t>Intangible assets</t>
+  </si>
+  <si>
+    <t>Date*metric</t>
+  </si>
+  <si>
+    <t>Repaymentrate</t>
   </si>
 </sst>
 </file>
@@ -636,19 +649,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -656,7 +671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -664,7 +679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>11</v>
       </c>
@@ -681,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -698,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>8</v>
       </c>
@@ -715,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>9</v>
       </c>
@@ -723,7 +738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -749,7 +764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -769,7 +784,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -792,7 +807,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -815,47 +830,47 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="D21" s="2"/>
     </row>
@@ -865,92 +880,217 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A3C72-8141-4CE1-9B29-33F3A1419413}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66504FB4-DA75-4B87-98E9-BDD1C8220F5C}">
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45688</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45716</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45747</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45777</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45808</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45869</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45900</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>45930</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>10000</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>46037</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4">
-        <v>100000</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>46902</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="4">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>46356</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
-        <v>20000</v>
-      </c>
-      <c r="D6">
-        <v>30</v>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45991</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>46022</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>46053</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>46081</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>46112</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>46142</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>46173</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>46203</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>46234</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>46265</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>46295</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>46326</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -959,6 +1099,100 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A3C72-8141-4CE1-9B29-33F3A1419413}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>46037</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>46902</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>46356</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>20000</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408AD00A-839B-4347-BBD4-5564B7B0FB9B}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -966,12 +1200,12 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -979,7 +1213,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -999,7 +1233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44926</v>
       </c>
@@ -1016,7 +1250,7 @@
         <v>3.0499999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44926</v>
       </c>
@@ -1033,7 +1267,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44926</v>
       </c>
@@ -1050,7 +1284,7 @@
         <v>3.1800000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44926</v>
       </c>
@@ -1067,7 +1301,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44926</v>
       </c>
@@ -1084,7 +1318,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44926</v>
       </c>
@@ -1101,7 +1335,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44926</v>
       </c>
@@ -1118,7 +1352,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44926</v>
       </c>
@@ -1138,7 +1372,7 @@
         <v>2.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44926</v>
       </c>
@@ -1158,7 +1392,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>46387</v>
       </c>
@@ -1175,7 +1409,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>46387</v>
       </c>
@@ -1192,7 +1426,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>46387</v>
       </c>
@@ -1209,7 +1443,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>46387</v>
       </c>
@@ -1226,7 +1460,7 @@
         <v>4.8600000000000004E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>46387</v>
       </c>
@@ -1243,7 +1477,7 @@
         <v>4.5499999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>46387</v>
       </c>
@@ -1260,7 +1494,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>46387</v>
       </c>
@@ -1277,7 +1511,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>46387</v>
       </c>
@@ -1297,7 +1531,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>46387</v>
       </c>
@@ -1315,165 +1549,6 @@
       </c>
       <c r="F20" s="3">
         <v>4.5499999999999999E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>46387</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>45658</v>
-      </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4">
-        <v>-100</v>
-      </c>
-      <c r="D4" s="1">
-        <v>45672</v>
-      </c>
-      <c r="E4" s="1">
-        <v>45930</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>45991</v>
-      </c>
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5">
-        <v>10000</v>
-      </c>
-      <c r="D5" s="1">
-        <v>46068</v>
-      </c>
-      <c r="E5" s="1">
-        <v>46158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>46172</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6">
-        <v>-500</v>
-      </c>
-      <c r="D6" s="1">
-        <v>45658</v>
-      </c>
-      <c r="E6" s="1">
-        <v>46022</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>46112</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7">
-        <v>600</v>
-      </c>
-      <c r="D7" s="1">
-        <v>45658</v>
-      </c>
-      <c r="E7" s="1">
-        <v>46022</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>46174</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8">
-        <v>5000</v>
-      </c>
-      <c r="D8" s="1">
-        <v>45717</v>
-      </c>
-      <c r="E8" s="1">
-        <v>45961</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>46174</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9">
-        <v>-4000</v>
-      </c>
-      <c r="D9" s="1">
-        <v>45717</v>
-      </c>
-      <c r="E9" s="1">
-        <v>45961</v>
       </c>
     </row>
   </sheetData>
@@ -1482,6 +1557,165 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45658</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4">
+        <v>-100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45672</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45930</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45991</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>46068</v>
+      </c>
+      <c r="E5" s="1">
+        <v>46158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>46172</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6">
+        <v>-500</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45658</v>
+      </c>
+      <c r="E6" s="1">
+        <v>46022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>46112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45658</v>
+      </c>
+      <c r="E7" s="1">
+        <v>46022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>46174</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45717</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45961</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>46174</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9">
+        <v>-4000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45717</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45961</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677DDE5-DC58-4FA0-9231-0F203A0C4FFF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1489,13 +1723,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.90625" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1503,7 +1737,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1511,58 +1745,8 @@
         <v>0.25700000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D314085B-29B2-4F1C-B0E6-FF11268580B0}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1570,23 +1754,73 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D314085B-29B2-4F1C-B0E6-FF11268580B0}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1594,7 +1828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1602,7 +1836,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1610,7 +1844,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1627,7 +1861,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45930</v>
       </c>
@@ -1644,7 +1878,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45991</v>
       </c>

</xml_diff>

<commit_message>
Implement manual input of repayment and prepayment in absolute amounts in balancesheetmutations
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A860A4C0-00F4-4A36-AC2E-89445045902E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74411F0C-D018-4589-965A-4E44C84E9E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
   <si>
     <t>Relative</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Nominal</t>
   </si>
   <si>
-    <t>ItemType</t>
-  </si>
-  <si>
     <t>Intangible assets</t>
   </si>
   <si>
@@ -259,6 +256,18 @@
   </si>
   <si>
     <t>Repaymentrate</t>
+  </si>
+  <si>
+    <t>SubItemType</t>
+  </si>
+  <si>
+    <t>Other loans</t>
+  </si>
+  <si>
+    <t>Repayment</t>
+  </si>
+  <si>
+    <t>Prepayment</t>
   </si>
 </sst>
 </file>
@@ -881,19 +890,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66504FB4-DA75-4B87-98E9-BDD1C8220F5C}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -901,195 +911,339 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>70</v>
       </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45688</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45716</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45747</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45777</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45808</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45838</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="4">
+        <v>50000</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45869</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45900</v>
       </c>
       <c r="B11" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45930</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45961</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45991</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>46022</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>46053</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>46081</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>46112</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>46142</v>
       </c>
       <c r="B19" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>46173</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>46203</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>46234</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>46265</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>46295</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>46326</v>
       </c>
       <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add rule for draw down and top up of undrawn balance. The draw down is based on the CCF column and can be overriden by scenario input, and the top up can be specified in scenario input as well.
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74411F0C-D018-4589-965A-4E44C84E9E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E38721B-8589-4071-9577-30AF0D4EDF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
   <si>
     <t>Relative</t>
   </si>
@@ -268,6 +268,18 @@
   </si>
   <si>
     <t>Prepayment</t>
+  </si>
+  <si>
+    <t>TopUp</t>
+  </si>
+  <si>
+    <t>DrawDown</t>
+  </si>
+  <si>
+    <t>TopUpRate</t>
+  </si>
+  <si>
+    <t>DrawDownRate</t>
   </si>
 </sst>
 </file>
@@ -890,20 +902,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66504FB4-DA75-4B87-98E9-BDD1C8220F5C}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -911,7 +924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -919,13 +932,25 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -933,317 +958,593 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
         <v>73</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45688</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45716</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45747</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45777</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
         <v>100000</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45808</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45838</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
         <v>50000</v>
       </c>
-      <c r="D9" s="4">
+      <c r="F9" s="4">
         <v>100000</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45869</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45900</v>
       </c>
       <c r="B11" s="2">
         <v>0.5</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45930</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45961</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45991</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>46022</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>46053</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>46081</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>46112</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>46142</v>
       </c>
       <c r="B19" s="2">
         <v>0.5</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>46173</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>46203</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>46234</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>46265</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>46295</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>46326</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make sure when adding new production items it is possible to introduce new labels
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_scenario.xlsx
+++ b/src/examples/scenarios/example_scenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E38721B-8589-4071-9577-30AF0D4EDF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0E6F0D-9A70-465A-A3E4-433E5AE02527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="81">
   <si>
     <t>Relative</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>DrawDownRate</t>
+  </si>
+  <si>
+    <t>Sub Item Type</t>
+  </si>
+  <si>
+    <t>New mortgage portfolio</t>
   </si>
 </sst>
 </file>
@@ -671,7 +677,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66504FB4-DA75-4B87-98E9-BDD1C8220F5C}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1555,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A3C72-8141-4CE1-9B29-33F3A1419413}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,7 +1573,7 @@
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1575,7 +1581,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1588,8 +1594,11 @@
       <c r="D2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45930</v>
       </c>
@@ -1603,42 +1612,59 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>46037</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="4">
         <v>100000</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>46902</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>200000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>46356</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>20000</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>30</v>
       </c>
     </row>

</xml_diff>